<commit_message>
Added UNIQUE constraints to db definition, changed classification_definition.
</commit_message>
<xml_diff>
--- a/mySQL_Create/aspects.xlsx
+++ b/mySQL_Create/aspects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Column name</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>DEFAULT NULL</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -566,15 +569,18 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -616,7 +622,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -629,11 +635,13 @@
       <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="F3" s="9"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -650,7 +658,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -669,7 +677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
@@ -682,11 +690,13 @@
       <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="F6" s="9"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
@@ -703,7 +713,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>21</v>
       </c>
@@ -720,7 +730,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -737,7 +747,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>

</xml_diff>